<commit_message>
MCannot use iterator when searching for a column number
</commit_message>
<xml_diff>
--- a/src/test/resources/df.xlsx
+++ b/src/test/resources/df.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="22">
   <si>
     <t xml:space="preserve">Mtcars</t>
   </si>
@@ -61,6 +61,9 @@
     <t xml:space="preserve">Iris</t>
   </si>
   <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sepal.Length</t>
   </si>
   <si>
@@ -97,6 +100,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -124,6 +128,7 @@
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -199,13 +204,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1329"/>
+  <dimension ref="A1:L1329"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L36" activeCellId="0" sqref="L36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="68.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.93"/>
@@ -1397,22 +1402,25 @@
       <c r="A36" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="L36" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1429,7 +1437,7 @@
         <v>0.2</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1446,7 +1454,7 @@
         <v>0.2</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1463,7 +1471,7 @@
         <v>0.2</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1480,7 +1488,7 @@
         <v>0.2</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1497,7 +1505,7 @@
         <v>0.2</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1514,7 +1522,7 @@
         <v>0.4</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1531,7 +1539,7 @@
         <v>0.3</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1548,7 +1556,7 @@
         <v>0.2</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1565,7 +1573,7 @@
         <v>0.2</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1582,7 +1590,7 @@
         <v>0.1</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1599,7 +1607,7 @@
         <v>0.2</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1616,7 +1624,7 @@
         <v>0.2</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1633,7 +1641,7 @@
         <v>0.1</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1650,7 +1658,7 @@
         <v>0.1</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1667,7 +1675,7 @@
         <v>0.2</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1684,7 +1692,7 @@
         <v>0.4</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1701,7 +1709,7 @@
         <v>0.4</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1718,7 +1726,7 @@
         <v>0.3</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1735,7 +1743,7 @@
         <v>0.3</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1752,7 +1760,7 @@
         <v>0.3</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1769,7 +1777,7 @@
         <v>0.2</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1786,7 +1794,7 @@
         <v>0.4</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1803,7 +1811,7 @@
         <v>0.2</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1820,7 +1828,7 @@
         <v>0.5</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1837,7 +1845,7 @@
         <v>0.2</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1854,7 +1862,7 @@
         <v>0.2</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1871,7 +1879,7 @@
         <v>0.4</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1888,7 +1896,7 @@
         <v>0.2</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1905,7 +1913,7 @@
         <v>0.2</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1922,7 +1930,7 @@
         <v>0.2</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1939,7 +1947,7 @@
         <v>0.2</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1956,7 +1964,7 @@
         <v>0.4</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1973,7 +1981,7 @@
         <v>0.1</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1990,7 +1998,7 @@
         <v>0.2</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2007,7 +2015,7 @@
         <v>0.2</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2024,7 +2032,7 @@
         <v>0.2</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2041,7 +2049,7 @@
         <v>0.2</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2058,7 +2066,7 @@
         <v>0.1</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2075,7 +2083,7 @@
         <v>0.2</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2092,7 +2100,7 @@
         <v>0.2</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2109,7 +2117,7 @@
         <v>0.3</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2126,7 +2134,7 @@
         <v>0.3</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2143,7 +2151,7 @@
         <v>0.2</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2160,7 +2168,7 @@
         <v>0.6</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2177,7 +2185,7 @@
         <v>0.4</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2194,7 +2202,7 @@
         <v>0.3</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2211,7 +2219,7 @@
         <v>0.2</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2228,7 +2236,7 @@
         <v>0.2</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2245,7 +2253,7 @@
         <v>0.2</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2262,7 +2270,7 @@
         <v>0.2</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2279,7 +2287,7 @@
         <v>1.4</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2296,7 +2304,7 @@
         <v>1.5</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2313,7 +2321,7 @@
         <v>1.5</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2330,7 +2338,7 @@
         <v>1.3</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2347,7 +2355,7 @@
         <v>1.5</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2364,7 +2372,7 @@
         <v>1.3</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2381,7 +2389,7 @@
         <v>1.6</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2398,7 +2406,7 @@
         <v>1</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2415,7 +2423,7 @@
         <v>1.3</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2432,7 +2440,7 @@
         <v>1.4</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2449,7 +2457,7 @@
         <v>1</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2466,7 +2474,7 @@
         <v>1.5</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2483,7 +2491,7 @@
         <v>1</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2500,7 +2508,7 @@
         <v>1.4</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2517,7 +2525,7 @@
         <v>1.3</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2534,7 +2542,7 @@
         <v>1.4</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2551,7 +2559,7 @@
         <v>1.5</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2568,7 +2576,7 @@
         <v>1</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2585,7 +2593,7 @@
         <v>1.5</v>
       </c>
       <c r="E106" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2602,7 +2610,7 @@
         <v>1.1</v>
       </c>
       <c r="E107" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2619,7 +2627,7 @@
         <v>1.8</v>
       </c>
       <c r="E108" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2636,7 +2644,7 @@
         <v>1.3</v>
       </c>
       <c r="E109" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2653,7 +2661,7 @@
         <v>1.5</v>
       </c>
       <c r="E110" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2670,7 +2678,7 @@
         <v>1.2</v>
       </c>
       <c r="E111" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2687,7 +2695,7 @@
         <v>1.3</v>
       </c>
       <c r="E112" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2704,7 +2712,7 @@
         <v>1.4</v>
       </c>
       <c r="E113" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2721,7 +2729,7 @@
         <v>1.4</v>
       </c>
       <c r="E114" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2738,7 +2746,7 @@
         <v>1.7</v>
       </c>
       <c r="E115" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2755,7 +2763,7 @@
         <v>1.5</v>
       </c>
       <c r="E116" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2772,7 +2780,7 @@
         <v>1</v>
       </c>
       <c r="E117" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2789,7 +2797,7 @@
         <v>1.1</v>
       </c>
       <c r="E118" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2806,7 +2814,7 @@
         <v>1</v>
       </c>
       <c r="E119" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2823,7 +2831,7 @@
         <v>1.2</v>
       </c>
       <c r="E120" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2840,7 +2848,7 @@
         <v>1.6</v>
       </c>
       <c r="E121" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2857,7 +2865,7 @@
         <v>1.5</v>
       </c>
       <c r="E122" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2874,7 +2882,7 @@
         <v>1.6</v>
       </c>
       <c r="E123" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2891,7 +2899,7 @@
         <v>1.5</v>
       </c>
       <c r="E124" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2908,7 +2916,7 @@
         <v>1.3</v>
       </c>
       <c r="E125" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2925,7 +2933,7 @@
         <v>1.3</v>
       </c>
       <c r="E126" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2942,7 +2950,7 @@
         <v>1.3</v>
       </c>
       <c r="E127" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2959,7 +2967,7 @@
         <v>1.2</v>
       </c>
       <c r="E128" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2976,7 +2984,7 @@
         <v>1.4</v>
       </c>
       <c r="E129" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2993,7 +3001,7 @@
         <v>1.2</v>
       </c>
       <c r="E130" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3010,7 +3018,7 @@
         <v>1</v>
       </c>
       <c r="E131" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3027,7 +3035,7 @@
         <v>1.3</v>
       </c>
       <c r="E132" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3044,7 +3052,7 @@
         <v>1.2</v>
       </c>
       <c r="E133" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3061,7 +3069,7 @@
         <v>1.3</v>
       </c>
       <c r="E134" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3078,7 +3086,7 @@
         <v>1.3</v>
       </c>
       <c r="E135" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3095,7 +3103,7 @@
         <v>1.1</v>
       </c>
       <c r="E136" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3112,7 +3120,7 @@
         <v>1.3</v>
       </c>
       <c r="E137" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3129,7 +3137,7 @@
         <v>2.5</v>
       </c>
       <c r="E138" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3146,7 +3154,7 @@
         <v>1.9</v>
       </c>
       <c r="E139" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3163,7 +3171,7 @@
         <v>2.1</v>
       </c>
       <c r="E140" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3180,7 +3188,7 @@
         <v>1.8</v>
       </c>
       <c r="E141" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3197,7 +3205,7 @@
         <v>2.2</v>
       </c>
       <c r="E142" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3214,7 +3222,7 @@
         <v>2.1</v>
       </c>
       <c r="E143" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3231,7 +3239,7 @@
         <v>1.7</v>
       </c>
       <c r="E144" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3248,7 +3256,7 @@
         <v>1.8</v>
       </c>
       <c r="E145" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3265,7 +3273,7 @@
         <v>1.8</v>
       </c>
       <c r="E146" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3282,7 +3290,7 @@
         <v>2.5</v>
       </c>
       <c r="E147" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3299,7 +3307,7 @@
         <v>2</v>
       </c>
       <c r="E148" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3316,7 +3324,7 @@
         <v>1.9</v>
       </c>
       <c r="E149" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3333,7 +3341,7 @@
         <v>2.1</v>
       </c>
       <c r="E150" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3350,7 +3358,7 @@
         <v>2</v>
       </c>
       <c r="E151" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3367,7 +3375,7 @@
         <v>2.4</v>
       </c>
       <c r="E152" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3384,7 +3392,7 @@
         <v>2.3</v>
       </c>
       <c r="E153" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3401,7 +3409,7 @@
         <v>1.8</v>
       </c>
       <c r="E154" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3418,7 +3426,7 @@
         <v>2.2</v>
       </c>
       <c r="E155" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3435,7 +3443,7 @@
         <v>2.3</v>
       </c>
       <c r="E156" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3452,7 +3460,7 @@
         <v>1.5</v>
       </c>
       <c r="E157" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3469,7 +3477,7 @@
         <v>2.3</v>
       </c>
       <c r="E158" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3486,7 +3494,7 @@
         <v>2</v>
       </c>
       <c r="E159" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3503,7 +3511,7 @@
         <v>2</v>
       </c>
       <c r="E160" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3520,7 +3528,7 @@
         <v>1.8</v>
       </c>
       <c r="E161" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3537,7 +3545,7 @@
         <v>2.1</v>
       </c>
       <c r="E162" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3554,7 +3562,7 @@
         <v>1.8</v>
       </c>
       <c r="E163" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3571,7 +3579,7 @@
         <v>1.8</v>
       </c>
       <c r="E164" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3588,7 +3596,7 @@
         <v>1.8</v>
       </c>
       <c r="E165" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3605,7 +3613,7 @@
         <v>2.1</v>
       </c>
       <c r="E166" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3622,7 +3630,7 @@
         <v>1.6</v>
       </c>
       <c r="E167" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3639,7 +3647,7 @@
         <v>1.9</v>
       </c>
       <c r="E168" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3656,7 +3664,7 @@
         <v>2</v>
       </c>
       <c r="E169" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3673,7 +3681,7 @@
         <v>2.2</v>
       </c>
       <c r="E170" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3690,7 +3698,7 @@
         <v>1.5</v>
       </c>
       <c r="E171" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3707,7 +3715,7 @@
         <v>1.4</v>
       </c>
       <c r="E172" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3724,7 +3732,7 @@
         <v>2.3</v>
       </c>
       <c r="E173" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3741,7 +3749,7 @@
         <v>2.4</v>
       </c>
       <c r="E174" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3758,7 +3766,7 @@
         <v>1.8</v>
       </c>
       <c r="E175" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3775,7 +3783,7 @@
         <v>1.8</v>
       </c>
       <c r="E176" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3792,7 +3800,7 @@
         <v>2.1</v>
       </c>
       <c r="E177" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3809,7 +3817,7 @@
         <v>2.4</v>
       </c>
       <c r="E178" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3826,7 +3834,7 @@
         <v>2.3</v>
       </c>
       <c r="E179" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3843,7 +3851,7 @@
         <v>1.9</v>
       </c>
       <c r="E180" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3860,7 +3868,7 @@
         <v>2.3</v>
       </c>
       <c r="E181" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3877,7 +3885,7 @@
         <v>2.5</v>
       </c>
       <c r="E182" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3894,7 +3902,7 @@
         <v>2.3</v>
       </c>
       <c r="E183" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3911,7 +3919,7 @@
         <v>1.9</v>
       </c>
       <c r="E184" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3928,7 +3936,7 @@
         <v>2</v>
       </c>
       <c r="E185" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3945,7 +3953,7 @@
         <v>2.3</v>
       </c>
       <c r="E186" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3962,7 +3970,7 @@
         <v>1.8</v>
       </c>
       <c r="E187" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>